<commit_message>
SYstem working, documentation created
</commit_message>
<xml_diff>
--- a/W-OP8/data/output/spreadsheets/Kodak_Lossless_True_Color_Image_Suite_tr0.1_max10_p30_g24_m0.05_x0.9_e2_t3_results.xlsx
+++ b/W-OP8/data/output/spreadsheets/Kodak_Lossless_True_Color_Image_Suite_tr0.1_max10_p30_g24_m0.05_x0.9_e2_t3_results.xlsx
@@ -495,9 +495,15 @@
       <c r="E2" t="n">
         <v>1179648</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>456214</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9.281697591145834</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -517,9 +523,15 @@
       <c r="E3" t="n">
         <v>1179648</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>394400</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.024088541666666</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -527,21 +539,22 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="D4">
-        <f>SUM(D2:D3)</f>
-        <v/>
-      </c>
-      <c r="E4">
-        <f>SUM(E2:E3)</f>
-        <v/>
-      </c>
-      <c r="F4">
-        <f>SUM(F2:F3)</f>
-        <v/>
-      </c>
-      <c r="G4">
-        <f>AVERAGE(G2:G3)</f>
-        <v/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="n">
+        <v>786432</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2359296</v>
+      </c>
+      <c r="F4" t="n">
+        <v>850614</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8.65289306640625</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -653,9 +666,15 @@
       <c r="E2" t="n">
         <v>1179648</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>500943</v>
+      </c>
+      <c r="G2" t="n">
+        <v>10.19171142578125</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -681,9 +700,15 @@
       <c r="E3" t="n">
         <v>1179648</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>478046</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9.725870768229166</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
@@ -709,9 +734,15 @@
       <c r="E4" t="n">
         <v>1179648</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>391854</v>
+      </c>
+      <c r="G4" t="n">
+        <v>7.9722900390625</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -737,9 +768,15 @@
       <c r="E5" t="n">
         <v>1179648</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>455834</v>
+      </c>
+      <c r="G5" t="n">
+        <v>9.273966471354166</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -765,9 +802,15 @@
       <c r="E6" t="n">
         <v>1179648</v>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>427699</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8.701558430989584</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
@@ -793,9 +836,15 @@
       <c r="E7" t="n">
         <v>1179648</v>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>341927</v>
+      </c>
+      <c r="G7" t="n">
+        <v>6.956522623697917</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -821,9 +870,15 @@
       <c r="E8" t="n">
         <v>1179648</v>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>522907</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10.63857014973958</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -849,9 +904,15 @@
       <c r="E9" t="n">
         <v>1179648</v>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>456200</v>
+      </c>
+      <c r="G9" t="n">
+        <v>9.281412760416666</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -877,9 +938,15 @@
       <c r="E10" t="n">
         <v>1179648</v>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>401282</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8.164103190104166</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
@@ -905,9 +972,15 @@
       <c r="E11" t="n">
         <v>1179648</v>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>483296</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9.832682291666666</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
@@ -933,9 +1006,15 @@
       <c r="E12" t="n">
         <v>1179648</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>433346</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.816446940104166</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
@@ -961,9 +1040,15 @@
       <c r="E13" t="n">
         <v>1179648</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>376433</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7.658548990885417</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -989,9 +1074,15 @@
       <c r="E14" t="n">
         <v>1179648</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>408138</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.3035888671875</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
@@ -1017,9 +1108,15 @@
       <c r="E15" t="n">
         <v>1179648</v>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>472926</v>
+      </c>
+      <c r="G15" t="n">
+        <v>9.6217041015625</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -1045,9 +1142,15 @@
       <c r="E16" t="n">
         <v>1179648</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>348655</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7.093404134114583</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
@@ -1073,9 +1176,15 @@
       <c r="E17" t="n">
         <v>1179648</v>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>404093</v>
+      </c>
+      <c r="G17" t="n">
+        <v>8.221293131510416</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -1101,9 +1210,15 @@
       <c r="E18" t="n">
         <v>1179648</v>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>376638</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7.6627197265625</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -1129,9 +1244,15 @@
       <c r="E19" t="n">
         <v>1179648</v>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>560798</v>
+      </c>
+      <c r="G19" t="n">
+        <v>11.40946451822917</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
@@ -1157,9 +1278,15 @@
       <c r="E20" t="n">
         <v>1179648</v>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>430179</v>
+      </c>
+      <c r="G20" t="n">
+        <v>8.75201416015625</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -1185,9 +1312,15 @@
       <c r="E21" t="n">
         <v>1179648</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>524120</v>
+      </c>
+      <c r="G21" t="n">
+        <v>10.66324869791667</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -1213,9 +1346,15 @@
       <c r="E22" t="n">
         <v>1179648</v>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>399513</v>
+      </c>
+      <c r="G22" t="n">
+        <v>8.12811279296875</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
@@ -1241,9 +1380,15 @@
       <c r="E23" t="n">
         <v>1179648</v>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>440634</v>
+      </c>
+      <c r="G23" t="n">
+        <v>8.9647216796875</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
@@ -1257,42 +1402,29 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="D24">
-        <f>SUM(D2:D23)</f>
-        <v/>
-      </c>
-      <c r="E24">
-        <f>SUM(E2:E23)</f>
-        <v/>
-      </c>
-      <c r="F24">
-        <f>SUM(F2:F23)</f>
-        <v/>
-      </c>
-      <c r="G24">
-        <f>AVERAGE(G2:G23)</f>
-        <v/>
-      </c>
-      <c r="I24">
-        <f>SUM(I2:I23)</f>
-        <v/>
-      </c>
-      <c r="J24">
-        <f>AVERAGE(J2:J23)</f>
-        <v/>
-      </c>
-      <c r="L24">
-        <f>SUM(L2:L23)</f>
-        <v/>
-      </c>
-      <c r="M24">
-        <f>AVERAGE(M2:M23)</f>
-        <v/>
-      </c>
-      <c r="N24">
-        <f>AVERAGE(N2:N23)</f>
-        <v/>
-      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="n">
+        <v>8650752</v>
+      </c>
+      <c r="E24" t="n">
+        <v>25952256</v>
+      </c>
+      <c r="F24" t="n">
+        <v>9635461</v>
+      </c>
+      <c r="G24" t="n">
+        <v>8.910634358723957</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1403,9 +1535,15 @@
       <c r="E2" t="n">
         <v>1179648</v>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>456214</v>
+      </c>
+      <c r="G2" t="n">
+        <v>9.281697591145834</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -1431,9 +1569,15 @@
       <c r="E3" t="n">
         <v>1179648</v>
       </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>394400</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.024088541666666</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
@@ -1459,9 +1603,15 @@
       <c r="E4" t="n">
         <v>1179648</v>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>500943</v>
+      </c>
+      <c r="G4" t="n">
+        <v>10.19171142578125</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
@@ -1487,9 +1637,15 @@
       <c r="E5" t="n">
         <v>1179648</v>
       </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>478046</v>
+      </c>
+      <c r="G5" t="n">
+        <v>9.725870768229166</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
@@ -1515,9 +1671,15 @@
       <c r="E6" t="n">
         <v>1179648</v>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>391854</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.9722900390625</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
@@ -1543,9 +1705,15 @@
       <c r="E7" t="n">
         <v>1179648</v>
       </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="F7" t="n">
+        <v>455834</v>
+      </c>
+      <c r="G7" t="n">
+        <v>9.273966471354166</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -1571,9 +1739,15 @@
       <c r="E8" t="n">
         <v>1179648</v>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>427699</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8.701558430989584</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
@@ -1599,9 +1773,15 @@
       <c r="E9" t="n">
         <v>1179648</v>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>341927</v>
+      </c>
+      <c r="G9" t="n">
+        <v>6.956522623697917</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
@@ -1627,9 +1807,15 @@
       <c r="E10" t="n">
         <v>1179648</v>
       </c>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>522907</v>
+      </c>
+      <c r="G10" t="n">
+        <v>10.63857014973958</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
@@ -1655,9 +1841,15 @@
       <c r="E11" t="n">
         <v>1179648</v>
       </c>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>456200</v>
+      </c>
+      <c r="G11" t="n">
+        <v>9.281412760416666</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
@@ -1683,9 +1875,15 @@
       <c r="E12" t="n">
         <v>1179648</v>
       </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
+      <c r="F12" t="n">
+        <v>401282</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.164103190104166</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
@@ -1711,9 +1909,15 @@
       <c r="E13" t="n">
         <v>1179648</v>
       </c>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
+      <c r="F13" t="n">
+        <v>483296</v>
+      </c>
+      <c r="G13" t="n">
+        <v>9.832682291666666</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
       <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
@@ -1739,9 +1943,15 @@
       <c r="E14" t="n">
         <v>1179648</v>
       </c>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
-      <c r="H14" t="inlineStr"/>
+      <c r="F14" t="n">
+        <v>433346</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.816446940104166</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
       <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
@@ -1767,9 +1977,15 @@
       <c r="E15" t="n">
         <v>1179648</v>
       </c>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
-      <c r="H15" t="inlineStr"/>
+      <c r="F15" t="n">
+        <v>376433</v>
+      </c>
+      <c r="G15" t="n">
+        <v>7.658548990885417</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
       <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
@@ -1795,9 +2011,15 @@
       <c r="E16" t="n">
         <v>1179648</v>
       </c>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
-      <c r="H16" t="inlineStr"/>
+      <c r="F16" t="n">
+        <v>408138</v>
+      </c>
+      <c r="G16" t="n">
+        <v>8.3035888671875</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0</v>
+      </c>
       <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
@@ -1823,9 +2045,15 @@
       <c r="E17" t="n">
         <v>1179648</v>
       </c>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
+      <c r="F17" t="n">
+        <v>472926</v>
+      </c>
+      <c r="G17" t="n">
+        <v>9.6217041015625</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
       <c r="I17" t="inlineStr"/>
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
@@ -1851,9 +2079,15 @@
       <c r="E18" t="n">
         <v>1179648</v>
       </c>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="F18" t="n">
+        <v>348655</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7.093404134114583</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0</v>
+      </c>
       <c r="I18" t="inlineStr"/>
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
@@ -1879,9 +2113,15 @@
       <c r="E19" t="n">
         <v>1179648</v>
       </c>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="F19" t="n">
+        <v>404093</v>
+      </c>
+      <c r="G19" t="n">
+        <v>8.221293131510416</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0</v>
+      </c>
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
@@ -1907,9 +2147,15 @@
       <c r="E20" t="n">
         <v>1179648</v>
       </c>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="F20" t="n">
+        <v>376638</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7.6627197265625</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0</v>
+      </c>
       <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
@@ -1935,9 +2181,15 @@
       <c r="E21" t="n">
         <v>1179648</v>
       </c>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="F21" t="n">
+        <v>560798</v>
+      </c>
+      <c r="G21" t="n">
+        <v>11.40946451822917</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
       <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
@@ -1963,9 +2215,15 @@
       <c r="E22" t="n">
         <v>1179648</v>
       </c>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="F22" t="n">
+        <v>430179</v>
+      </c>
+      <c r="G22" t="n">
+        <v>8.75201416015625</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
       <c r="I22" t="inlineStr"/>
       <c r="J22" t="inlineStr"/>
       <c r="K22" t="inlineStr"/>
@@ -1991,9 +2249,15 @@
       <c r="E23" t="n">
         <v>1179648</v>
       </c>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="F23" t="n">
+        <v>524120</v>
+      </c>
+      <c r="G23" t="n">
+        <v>10.66324869791667</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0</v>
+      </c>
       <c r="I23" t="inlineStr"/>
       <c r="J23" t="inlineStr"/>
       <c r="K23" t="inlineStr"/>
@@ -2019,9 +2283,15 @@
       <c r="E24" t="n">
         <v>1179648</v>
       </c>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="F24" t="n">
+        <v>399513</v>
+      </c>
+      <c r="G24" t="n">
+        <v>8.12811279296875</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0</v>
+      </c>
       <c r="I24" t="inlineStr"/>
       <c r="J24" t="inlineStr"/>
       <c r="K24" t="inlineStr"/>
@@ -2047,9 +2317,15 @@
       <c r="E25" t="n">
         <v>1179648</v>
       </c>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
-      <c r="H25" t="inlineStr"/>
+      <c r="F25" t="n">
+        <v>440634</v>
+      </c>
+      <c r="G25" t="n">
+        <v>8.9647216796875</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
       <c r="I25" t="inlineStr"/>
       <c r="J25" t="inlineStr"/>
       <c r="K25" t="inlineStr"/>
@@ -2063,42 +2339,29 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="D26">
-        <f>SUM(D2:D25)</f>
-        <v/>
-      </c>
-      <c r="E26">
-        <f>SUM(E2:E25)</f>
-        <v/>
-      </c>
-      <c r="F26">
-        <f>SUM(F2:F25)</f>
-        <v/>
-      </c>
-      <c r="G26">
-        <f>AVERAGE(G2:G25)</f>
-        <v/>
-      </c>
-      <c r="I26">
-        <f>SUM(I2:I25)</f>
-        <v/>
-      </c>
-      <c r="J26">
-        <f>AVERAGE(J2:J25)</f>
-        <v/>
-      </c>
-      <c r="L26">
-        <f>SUM(L2:L25)</f>
-        <v/>
-      </c>
-      <c r="M26">
-        <f>AVERAGE(M2:M25)</f>
-        <v/>
-      </c>
-      <c r="N26">
-        <f>AVERAGE(N2:N25)</f>
-        <v/>
-      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="n">
+        <v>9437184</v>
+      </c>
+      <c r="E26" t="n">
+        <v>28311552</v>
+      </c>
+      <c r="F26" t="n">
+        <v>10486075</v>
+      </c>
+      <c r="G26" t="n">
+        <v>8.889155917697481</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>